<commit_message>
Dashboard assessment and other commits
</commit_message>
<xml_diff>
--- a/data/CreateDashboard.xlsx
+++ b/data/CreateDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/11ed534c7d8b8a9a/Desktop/SeleniumPreparation/Framework_with_ThreadLocal/Framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{EECA046F-C6B9-465F-A6F5-3732B5E47AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{757B7839-2EE0-4F16-ABF9-63690D43CA17}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{EECA046F-C6B9-465F-A6F5-3732B5E47AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63BD752D-019D-40B4-BFAF-FED6910BBDF6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Sankar</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -120,6 +126,10 @@
 </file>
 
 <file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -386,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +407,7 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +420,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -424,8 +437,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -437,6 +453,9 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>